<commit_message>
added data driven test cases
</commit_message>
<xml_diff>
--- a/testData/userData.xlsx
+++ b/testData/userData.xlsx
@@ -13,25 +13,25 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
-    <t xml:space="preserve"> id</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> username</t>
-  </si>
-  <si>
-    <t>firstName</t>
-  </si>
-  <si>
-    <t>lastName</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>phone</t>
+    <t xml:space="preserve"> UserId</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> UserName</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Phone</t>
   </si>
   <si>
     <t>testuser1</t>

</xml_diff>